<commit_message>
documentation, and xlsx file browse
</commit_message>
<xml_diff>
--- a/sample_4/Sample_4.xlsx
+++ b/sample_4/Sample_4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zderoche\DocumentsLocal\git\zemax-lens-xlsx-import\sample_4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zderoche\DocumentsLocal\git\zemax-xlsx-import\sample_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83D6EF5F-8ADC-4361-B390-254B721595E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CB92BEF-6E5D-48FB-A25B-5E014D80639C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7725" yWindow="-16065" windowWidth="23250" windowHeight="13890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-5115" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LensData" sheetId="5" r:id="rId1"/>
@@ -244,9 +244,6 @@
     <t>FPL51</t>
   </si>
   <si>
-    <t>ALL_PREF_CDGM+SCHOTT_ONLY</t>
-  </si>
-  <si>
     <t>OHARA</t>
   </si>
   <si>
@@ -254,6 +251,9 @@
   </si>
   <si>
     <t>infinity</t>
+  </si>
+  <si>
+    <t>SCHOTT</t>
   </si>
 </sst>
 </file>
@@ -595,7 +595,7 @@
   <dimension ref="A1:M38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -655,13 +655,13 @@
         <v>32</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>50</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -695,7 +695,7 @@
         <v>56</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -729,7 +729,7 @@
         <v>57</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -749,7 +749,7 @@
         <v>58</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -783,7 +783,7 @@
         <v>59</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -817,7 +817,7 @@
         <v>60</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -865,7 +865,7 @@
         <v>61</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:13">
@@ -899,7 +899,7 @@
         <v>62</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:13">
@@ -919,7 +919,7 @@
         <v>63</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:13">
@@ -939,7 +939,7 @@
         <v>64</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:13">
@@ -973,7 +973,7 @@
         <v>65</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:13">
@@ -993,7 +993,7 @@
         <v>58</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:13">

</xml_diff>